<commit_message>
Added literacy data to main statewise data, added linear regression model IPyNB Notebook
</commit_message>
<xml_diff>
--- a/Data Processed/Statewise Data.xlsx
+++ b/Data Processed/Statewise Data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="131">
   <si>
     <t>ANDAMAN AND NICOBAR ISLANDS</t>
   </si>
@@ -1915,13 +1915,16 @@
   </si>
   <si>
     <t>2015 Inflatn January</t>
+  </si>
+  <si>
+    <t>2010-2015 Litracy Rate State</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1963,6 +1966,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -2011,7 +2021,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2068,6 +2078,13 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -2372,10 +2389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AY73"/>
+  <dimension ref="A1:AZ73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ709" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2387,7 +2404,7 @@
     <col min="10" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:52" ht="60" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>33</v>
       </c>
@@ -2418,125 +2435,128 @@
       <c r="L1" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="M1" s="19" t="s">
+      <c r="M1" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="N1" s="19" t="s">
+      <c r="N1" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="O1" s="19" t="s">
+      <c r="O1" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="V1" t="s">
+      <c r="V1" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="W1" t="s">
+      <c r="W1" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="X1" t="s">
+      <c r="X1" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Y1" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="Z1" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AA1" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AB1" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AC1" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AD1" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AE1" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AF1" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AG1" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AH1" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AI1" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AJ1" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AK1" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AL1" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AM1" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AN1" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AO1" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AP1" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AQ1" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AR1" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AS1" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AT1" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AU1" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AV1" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AW1" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AX1" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AY1" s="21" t="s">
         <v>123</v>
       </c>
+      <c r="AZ1" s="21" t="s">
+        <v>130</v>
+      </c>
     </row>
-    <row r="2" spans="1:51" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:52" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2688,7 +2708,7 @@
         <v>126.3</v>
       </c>
     </row>
-    <row r="3" spans="1:51" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:52" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -2839,8 +2859,11 @@
       <c r="AY3">
         <v>130.9</v>
       </c>
+      <c r="AZ3" s="20">
+        <v>68.5</v>
+      </c>
     </row>
-    <row r="4" spans="1:51" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:52" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -2991,8 +3014,9 @@
       <c r="AY4" t="s">
         <v>112</v>
       </c>
+      <c r="AZ4" s="20"/>
     </row>
-    <row r="5" spans="1:51" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:52" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -3143,8 +3167,11 @@
       <c r="AY5">
         <v>125.7</v>
       </c>
+      <c r="AZ5" s="20">
+        <v>63.9</v>
+      </c>
     </row>
-    <row r="6" spans="1:51" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:52" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -3295,8 +3322,11 @@
       <c r="AY6">
         <v>129.1</v>
       </c>
+      <c r="AZ6" s="20">
+        <v>68.099999999999994</v>
+      </c>
     </row>
-    <row r="7" spans="1:51" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:52" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -3447,8 +3477,9 @@
       <c r="AY7">
         <v>121.5</v>
       </c>
+      <c r="AZ7" s="20"/>
     </row>
-    <row r="8" spans="1:51" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:52" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -3599,8 +3630,11 @@
       <c r="AY8">
         <v>130.19999999999999</v>
       </c>
+      <c r="AZ8" s="20">
+        <v>64.8</v>
+      </c>
     </row>
-    <row r="9" spans="1:51" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:52" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -3751,8 +3785,11 @@
       <c r="AY9">
         <v>122.4</v>
       </c>
+      <c r="AZ9" s="20">
+        <v>73.2</v>
+      </c>
     </row>
-    <row r="10" spans="1:51" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:52" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -3903,8 +3940,9 @@
       <c r="AY10">
         <v>127.7</v>
       </c>
+      <c r="AZ10" s="20"/>
     </row>
-    <row r="11" spans="1:51" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:52" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -4055,8 +4093,11 @@
       <c r="AY11">
         <v>124.3</v>
       </c>
+      <c r="AZ11" s="20">
+        <v>68.7</v>
+      </c>
     </row>
-    <row r="12" spans="1:51" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:52" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -4207,8 +4248,11 @@
       <c r="AY12">
         <v>122.4</v>
       </c>
+      <c r="AZ12" s="20">
+        <v>68.599999999999994</v>
+      </c>
     </row>
-    <row r="13" spans="1:51" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:52" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -4359,8 +4403,11 @@
       <c r="AY13">
         <v>125</v>
       </c>
+      <c r="AZ13" s="20">
+        <v>71.599999999999994</v>
+      </c>
     </row>
-    <row r="14" spans="1:51" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:52" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -4511,8 +4558,11 @@
       <c r="AY14">
         <v>124.4</v>
       </c>
+      <c r="AZ14" s="20">
+        <v>72.599999999999994</v>
+      </c>
     </row>
-    <row r="15" spans="1:51" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:52" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -4663,8 +4713,11 @@
       <c r="AY15">
         <v>126.3</v>
       </c>
+      <c r="AZ15" s="20">
+        <v>66.599999999999994</v>
+      </c>
     </row>
-    <row r="16" spans="1:51" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:52" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -4815,8 +4868,11 @@
       <c r="AY16">
         <v>131</v>
       </c>
+      <c r="AZ16" s="20">
+        <v>68.8</v>
+      </c>
     </row>
-    <row r="17" spans="1:51" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:52" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
@@ -4967,8 +5023,11 @@
       <c r="AY17">
         <v>126.2</v>
       </c>
+      <c r="AZ17" s="20">
+        <v>74.900000000000006</v>
+      </c>
     </row>
-    <row r="18" spans="1:51" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:52" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
@@ -5119,8 +5178,11 @@
       <c r="AY18">
         <v>125.3</v>
       </c>
+      <c r="AZ18" s="20">
+        <v>64.2</v>
+      </c>
     </row>
-    <row r="19" spans="1:51" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:52" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
@@ -5271,8 +5333,11 @@
       <c r="AY19">
         <v>123.5</v>
       </c>
+      <c r="AZ19" s="20">
+        <v>71.599999999999994</v>
+      </c>
     </row>
-    <row r="20" spans="1:51" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:52" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
@@ -5423,8 +5488,9 @@
       <c r="AY20">
         <v>117.2</v>
       </c>
+      <c r="AZ20" s="20"/>
     </row>
-    <row r="21" spans="1:51" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:52" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
@@ -5575,8 +5641,9 @@
       <c r="AY21">
         <v>133.80000000000001</v>
       </c>
+      <c r="AZ21" s="20"/>
     </row>
-    <row r="22" spans="1:51" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:52" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
@@ -5727,8 +5794,9 @@
       <c r="AY22">
         <v>127.6</v>
       </c>
+      <c r="AZ22" s="20"/>
     </row>
-    <row r="23" spans="1:51" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:52" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
@@ -5879,8 +5947,9 @@
       <c r="AY23">
         <v>130.19999999999999</v>
       </c>
+      <c r="AZ23" s="20"/>
     </row>
-    <row r="24" spans="1:51" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:52" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
@@ -6031,8 +6100,11 @@
       <c r="AY24">
         <v>130.1</v>
       </c>
+      <c r="AZ24" s="20">
+        <v>65.8</v>
+      </c>
     </row>
-    <row r="25" spans="1:51" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:52" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
@@ -6183,8 +6255,9 @@
       <c r="AY25">
         <v>130.4</v>
       </c>
+      <c r="AZ25" s="20"/>
     </row>
-    <row r="26" spans="1:51" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:52" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
@@ -6335,8 +6408,11 @@
       <c r="AY26">
         <v>122.2</v>
       </c>
+      <c r="AZ26" s="20">
+        <v>71.599999999999994</v>
+      </c>
     </row>
-    <row r="27" spans="1:51" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:52" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>25</v>
       </c>
@@ -6487,8 +6563,11 @@
       <c r="AY27">
         <v>127</v>
       </c>
+      <c r="AZ27" s="20">
+        <v>67.7</v>
+      </c>
     </row>
-    <row r="28" spans="1:51" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:52" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
@@ -6639,8 +6718,9 @@
       <c r="AY28">
         <v>126.3</v>
       </c>
+      <c r="AZ28" s="20"/>
     </row>
-    <row r="29" spans="1:51" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:52" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>27</v>
       </c>
@@ -6791,8 +6871,11 @@
       <c r="AY29">
         <v>129.1</v>
       </c>
+      <c r="AZ29" s="20">
+        <v>70.599999999999994</v>
+      </c>
     </row>
-    <row r="30" spans="1:51" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:52" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>28</v>
       </c>
@@ -6943,8 +7026,9 @@
       <c r="AY30">
         <v>125.3</v>
       </c>
+      <c r="AZ30" s="20"/>
     </row>
-    <row r="31" spans="1:51" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:52" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>29</v>
       </c>
@@ -7095,8 +7179,9 @@
       <c r="AY31">
         <v>133</v>
       </c>
+      <c r="AZ31" s="20"/>
     </row>
-    <row r="32" spans="1:51" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:52" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
@@ -7247,8 +7332,11 @@
       <c r="AY32">
         <v>125.6</v>
       </c>
+      <c r="AZ32" s="20">
+        <v>64.099999999999994</v>
+      </c>
     </row>
-    <row r="33" spans="1:51" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:52" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
@@ -7399,8 +7487,11 @@
       <c r="AY33">
         <v>120.9</v>
       </c>
+      <c r="AZ33" s="20">
+        <v>71.7</v>
+      </c>
     </row>
-    <row r="34" spans="1:51" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:52" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
@@ -7551,66 +7642,69 @@
       <c r="AY34">
         <v>124.3</v>
       </c>
+      <c r="AZ34" s="20">
+        <v>70.2</v>
+      </c>
     </row>
-    <row r="36" spans="1:51" ht="47.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:51" ht="47.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:51" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:52" ht="47.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:52" ht="47.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:52" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H40" s="5"/>
       <c r="I40" s="14"/>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
       <c r="L40" s="7"/>
     </row>
-    <row r="41" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:52" x14ac:dyDescent="0.25">
       <c r="H41" s="9"/>
       <c r="I41" s="15"/>
       <c r="J41" s="9"/>
       <c r="K41" s="9"/>
       <c r="L41" s="6"/>
     </row>
-    <row r="42" spans="1:51" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:52" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H42" s="9"/>
       <c r="I42" s="15"/>
       <c r="J42" s="9"/>
       <c r="K42" s="9"/>
       <c r="L42" s="6"/>
     </row>
-    <row r="43" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:52" x14ac:dyDescent="0.25">
       <c r="H43" s="9"/>
       <c r="I43" s="15"/>
       <c r="J43" s="9"/>
       <c r="K43" s="9"/>
       <c r="L43" s="6"/>
     </row>
-    <row r="44" spans="1:51" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:52" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H44" s="9"/>
       <c r="I44" s="15"/>
       <c r="J44" s="9"/>
       <c r="K44" s="9"/>
       <c r="L44" s="6"/>
     </row>
-    <row r="45" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:52" x14ac:dyDescent="0.25">
       <c r="H45" s="9"/>
       <c r="I45" s="15"/>
       <c r="J45" s="9"/>
       <c r="K45" s="9"/>
       <c r="L45" s="6"/>
     </row>
-    <row r="46" spans="1:51" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:52" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H46" s="9"/>
       <c r="I46" s="15"/>
       <c r="J46" s="9"/>
       <c r="K46" s="9"/>
       <c r="L46" s="6"/>
     </row>
-    <row r="47" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:52" x14ac:dyDescent="0.25">
       <c r="H47" s="9"/>
       <c r="I47" s="15"/>
       <c r="J47" s="9"/>
       <c r="K47" s="9"/>
       <c r="L47" s="6"/>
     </row>
-    <row r="48" spans="1:51" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:52" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H48" s="3"/>
       <c r="I48" s="15"/>
       <c r="J48" s="9"/>
@@ -7811,6 +7905,7 @@
     <hyperlink ref="H1" r:id="rId4" location="cite_note-Rural_Urban_distribution-15" display="https://en.wikipedia.org/wiki/List_of_states_and_union_territories_of_India_by_population - cite_note-Rural_Urban_distribution-15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
More datasets and books
</commit_message>
<xml_diff>
--- a/Data Processed/Statewise Data.xlsx
+++ b/Data Processed/Statewise Data.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -2392,7 +2392,7 @@
   <dimension ref="A1:AZ73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+      <selection activeCell="A2" sqref="A2:A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2560,6 +2560,10 @@
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="B2">
+        <f>C2/F2</f>
+        <v>1.1813293537995073</v>
+      </c>
       <c r="C2" s="1">
         <v>448839</v>
       </c>
@@ -2712,6 +2716,10 @@
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="B3">
+        <f>C3/F3</f>
+        <v>0.82433919234166197</v>
+      </c>
       <c r="C3" s="1">
         <v>40711474</v>
       </c>
@@ -2866,6 +2874,10 @@
     <row r="4" spans="1:52" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
+      </c>
+      <c r="B4">
+        <f>C4/F4</f>
+        <v>0.89239417305373669</v>
       </c>
       <c r="C4" s="1">
         <v>1233834</v>
@@ -3020,6 +3032,10 @@
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="B5">
+        <f>C5/F5</f>
+        <v>0.49576197993973037</v>
+      </c>
       <c r="C5" s="1">
         <v>15452540</v>
       </c>
@@ -3175,6 +3191,10 @@
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="B6">
+        <f>C6/F6</f>
+        <v>0.25976666148353278</v>
+      </c>
       <c r="C6" s="1">
         <v>26964984</v>
       </c>
@@ -3329,6 +3349,10 @@
     <row r="7" spans="1:52" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="B7">
+        <f>C7/F7</f>
+        <v>2.0943322753327966</v>
       </c>
       <c r="C7" s="1">
         <v>2210463</v>
@@ -3483,6 +3507,10 @@
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="B8">
+        <f>C8/F8</f>
+        <v>0.7148709821960646</v>
+      </c>
       <c r="C8" s="1">
         <v>18257945</v>
       </c>
@@ -3638,6 +3666,10 @@
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="B9">
+        <f>C9/F9</f>
+        <v>2.3404203052655475</v>
+      </c>
       <c r="C9" s="1">
         <v>39290838</v>
       </c>
@@ -3792,6 +3824,10 @@
     <row r="10" spans="1:52" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="B10">
+        <f>C10/F10</f>
+        <v>2.165600734844686</v>
       </c>
       <c r="C10" s="1">
         <v>3156846</v>
@@ -3946,6 +3982,10 @@
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="B11">
+        <f>C11/F11</f>
+        <v>1.2160313885081566</v>
+      </c>
       <c r="C11" s="1">
         <v>73428387</v>
       </c>
@@ -4101,6 +4141,10 @@
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="B12">
+        <f>C12/F12</f>
+        <v>1.3678784049954322</v>
+      </c>
       <c r="C12" s="1">
         <v>34679932</v>
       </c>
@@ -4256,6 +4300,10 @@
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="B13">
+        <f>C13/F13</f>
+        <v>1.2068680747988012</v>
+      </c>
       <c r="C13" s="1">
         <v>8284669</v>
       </c>
@@ -4411,6 +4459,10 @@
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="B14">
+        <f>C14/F14</f>
+        <v>0.67826920008931446</v>
+      </c>
       <c r="C14" s="1">
         <v>8511550</v>
       </c>
@@ -4566,6 +4618,10 @@
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="B15">
+        <f>C15/F15</f>
+        <v>0.50298811772213747</v>
+      </c>
       <c r="C15" s="1">
         <v>16581626</v>
       </c>
@@ -4721,6 +4777,10 @@
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="B16">
+        <f>C16/F16</f>
+        <v>1.1530205999263479</v>
+      </c>
       <c r="C16" s="1">
         <v>70484961</v>
       </c>
@@ -4876,6 +4936,10 @@
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="B17">
+        <f>C17/F17</f>
+        <v>1.2063772211525827</v>
+      </c>
       <c r="C17" s="1">
         <v>40278133</v>
       </c>
@@ -5031,6 +5095,10 @@
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="B18">
+        <f>C18/F18</f>
+        <v>0.50295618041734591</v>
+      </c>
       <c r="C18" s="1">
         <v>36513394</v>
       </c>
@@ -5186,6 +5254,10 @@
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="B19">
+        <f>C19/F19</f>
+        <v>1.2917706759593401</v>
+      </c>
       <c r="C19" s="1">
         <v>145160110</v>
       </c>
@@ -5340,6 +5412,10 @@
     <row r="20" spans="1:52" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>18</v>
+      </c>
+      <c r="B20">
+        <f>C20/F20</f>
+        <v>0.5186023287906778</v>
       </c>
       <c r="C20" s="1">
         <v>1411509</v>
@@ -5494,6 +5570,10 @@
       <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="B21">
+        <f>C21/F21</f>
+        <v>0.69924632431704781</v>
+      </c>
       <c r="C21" s="1">
         <v>2072571</v>
       </c>
@@ -5647,6 +5727,10 @@
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="B22">
+        <f>C22/F22</f>
+        <v>0.82844216481181732</v>
+      </c>
       <c r="C22" s="1">
         <v>903842</v>
       </c>
@@ -5800,6 +5884,10 @@
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="B23">
+        <f>C23/F23</f>
+        <v>0.69638372575610852</v>
+      </c>
       <c r="C23" s="1">
         <v>1379259</v>
       </c>
@@ -5953,6 +6041,10 @@
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="B24">
+        <f>C24/F24</f>
+        <v>0.63386952761125026</v>
+      </c>
       <c r="C24" s="1">
         <v>26589152</v>
       </c>
@@ -6107,6 +6199,10 @@
     <row r="25" spans="1:52" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>23</v>
+      </c>
+      <c r="B25">
+        <f>C25/F25</f>
+        <v>1.5404423109065428</v>
       </c>
       <c r="C25" s="1">
         <v>1917025</v>
@@ -6261,6 +6357,10 @@
       <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="B26">
+        <f>C26/F26</f>
+        <v>1.0808806638811479</v>
+      </c>
       <c r="C26" s="1">
         <v>29944973</v>
       </c>
@@ -6416,6 +6516,10 @@
       <c r="A27" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="B27">
+        <f>C27/F27</f>
+        <v>0.70857331570685667</v>
+      </c>
       <c r="C27" s="1">
         <v>48623018</v>
       </c>
@@ -6570,6 +6674,10 @@
     <row r="28" spans="1:52" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>26</v>
+      </c>
+      <c r="B28">
+        <f>C28/F28</f>
+        <v>1.9934653967167362</v>
       </c>
       <c r="C28" s="1">
         <v>1211405</v>
@@ -6724,6 +6832,10 @@
       <c r="A29" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="B29">
+        <f>C29/F29</f>
+        <v>1.1810200807169962</v>
+      </c>
       <c r="C29" s="1">
         <v>85197558</v>
       </c>
@@ -6878,6 +6990,10 @@
     <row r="30" spans="1:52" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>28</v>
+      </c>
+      <c r="B30">
+        <f>C30/F30</f>
+        <v>1.1051080154518025</v>
       </c>
       <c r="C30" s="1">
         <v>38995678</v>
@@ -7032,6 +7148,10 @@
       <c r="A31" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="B31">
+        <f>C31/F31</f>
+        <v>0.6215993213897345</v>
+      </c>
       <c r="C31" s="1">
         <v>2281911</v>
       </c>
@@ -7185,6 +7305,10 @@
       <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="B32">
+        <f>C32/F32</f>
+        <v>0.40141148739156207</v>
+      </c>
       <c r="C32" s="1">
         <v>80206969</v>
       </c>
@@ -7340,6 +7464,10 @@
       <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="B33">
+        <f>C33/F33</f>
+        <v>1.3263382358290488</v>
+      </c>
       <c r="C33" s="1">
         <v>13418235</v>
       </c>
@@ -7494,6 +7622,10 @@
     <row r="34" spans="1:52" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>32</v>
+      </c>
+      <c r="B34">
+        <f>C34/F34</f>
+        <v>0.73755665931337366</v>
       </c>
       <c r="C34" s="1">
         <v>67374131</v>

</xml_diff>